<commit_message>
v1 das mascaras de codigo da taurus e v1 de regex
</commit_message>
<xml_diff>
--- a/data-raw/colunas_finais.xlsx
+++ b/data-raw/colunas_finais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fernando\OneDrive\Documentos\projetos.R\isdp.armas\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BB7C60-704E-48BE-A0C0-90AE8C173C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8E8863-D5C1-4901-9BF1-43517BBA98D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{103D21A8-1D66-400B-A497-781683E3805A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="85">
   <si>
     <t>x</t>
   </si>
@@ -218,12 +218,6 @@
     <t>DESCR_ARMA_FOGO</t>
   </si>
   <si>
-    <t>COLUNA</t>
-  </si>
-  <si>
-    <t>BASE FATOS</t>
-  </si>
-  <si>
     <t>BASE ARMAS</t>
   </si>
   <si>
@@ -257,10 +251,46 @@
     <t>FLAG_ARMA_ARTESANAL</t>
   </si>
   <si>
-    <t>1 Se for possível identificar que é uma arma artesanal, 0 em caso contrário. Vai adotar uma série de critérios</t>
-  </si>
-  <si>
     <t>id_municipio_ibge</t>
+  </si>
+  <si>
+    <t>BASE OCORRENCIAS</t>
+  </si>
+  <si>
+    <t>COLUNA BASE 2</t>
+  </si>
+  <si>
+    <t>COLUNA BASE 1</t>
+  </si>
+  <si>
+    <t>1 Se for possível identificar que é uma arma artesanal, 0 em caso contrário. Vai adotar uma série de critérios. Ideia: usar a descrição e na coluna de marca também tem padrões para considerarmos</t>
+  </si>
+  <si>
+    <t>ANO_FABRICACAO</t>
+  </si>
+  <si>
+    <t>Classificação textual em "pistola", "metralhadora" etc</t>
+  </si>
+  <si>
+    <t>Aqui calibre será padronizado na versão final</t>
+  </si>
+  <si>
+    <t>Vamos padronizar as rubricas em classes específicas relevantes</t>
+  </si>
+  <si>
+    <t>Vamos padronizar os tipos de local</t>
+  </si>
+  <si>
+    <t>Vamos tentar incluir as latlons usando as tecnologias da OpenStreetMap</t>
+  </si>
+  <si>
+    <t>A ideia é mexer nesse dado o mínimo possível. Se estiver vazio preencher, mas se não estiver manter o que já está lá</t>
+  </si>
+  <si>
+    <t>As marcas serão padronizadas</t>
+  </si>
+  <si>
+    <t>A ideia é obter esse dado vindo do id da arma</t>
   </si>
 </sst>
 </file>
@@ -296,9 +326,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,16 +668,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E11677A-1829-481E-A567-918BBA26AEF0}">
-  <dimension ref="B1:G64"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
@@ -650,28 +686,31 @@
     <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
       <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>62</v>
       </c>
-      <c r="E1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>64</v>
       </c>
-      <c r="G1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
@@ -684,10 +723,10 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -701,10 +740,10 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -718,10 +757,10 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -735,10 +774,10 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -752,10 +791,10 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -769,10 +808,10 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -786,10 +825,10 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -803,10 +842,10 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -820,10 +859,10 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -837,10 +876,10 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -854,10 +893,10 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -865,10 +904,10 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -876,10 +915,10 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -887,10 +926,10 @@
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>15</v>
       </c>
@@ -898,10 +937,10 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -909,10 +948,10 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -920,10 +959,10 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>18</v>
       </c>
@@ -931,10 +970,10 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>19</v>
       </c>
@@ -942,10 +981,10 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>20</v>
       </c>
@@ -953,10 +992,10 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -964,10 +1003,10 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>22</v>
       </c>
@@ -975,10 +1014,10 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>23</v>
       </c>
@@ -986,10 +1025,10 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>24</v>
       </c>
@@ -997,10 +1036,10 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>25</v>
       </c>
@@ -1008,10 +1047,13 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>26</v>
       </c>
@@ -1019,10 +1061,11 @@
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>27</v>
       </c>
@@ -1030,10 +1073,11 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>28</v>
       </c>
@@ -1041,10 +1085,10 @@
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>29</v>
       </c>
@@ -1052,10 +1096,13 @@
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>30</v>
       </c>
@@ -1063,10 +1110,11 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>31</v>
       </c>
@@ -1074,10 +1122,10 @@
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>32</v>
       </c>
@@ -1085,10 +1133,10 @@
         <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>33</v>
       </c>
@@ -1096,10 +1144,10 @@
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>34</v>
       </c>
@@ -1107,10 +1155,13 @@
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>35</v>
       </c>
@@ -1118,10 +1169,10 @@
         <v>0</v>
       </c>
       <c r="F36" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>36</v>
       </c>
@@ -1129,18 +1180,21 @@
         <v>0</v>
       </c>
       <c r="F37" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>37</v>
       </c>
+      <c r="D38" t="s">
+        <v>0</v>
+      </c>
       <c r="F38" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>38</v>
       </c>
@@ -1148,10 +1202,10 @@
         <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>39</v>
       </c>
@@ -1159,10 +1213,10 @@
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>40</v>
       </c>
@@ -1170,10 +1224,10 @@
         <v>0</v>
       </c>
       <c r="F41" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>41</v>
       </c>
@@ -1181,10 +1235,10 @@
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>42</v>
       </c>
@@ -1192,10 +1246,10 @@
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>43</v>
       </c>
@@ -1203,10 +1257,10 @@
         <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>44</v>
       </c>
@@ -1214,10 +1268,10 @@
         <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>45</v>
       </c>
@@ -1225,10 +1279,10 @@
         <v>0</v>
       </c>
       <c r="F46" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>46</v>
       </c>
@@ -1236,10 +1290,10 @@
         <v>0</v>
       </c>
       <c r="F47" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>47</v>
       </c>
@@ -1247,7 +1301,7 @@
         <v>0</v>
       </c>
       <c r="F48" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
@@ -1258,7 +1312,7 @@
         <v>0</v>
       </c>
       <c r="F49" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
@@ -1269,7 +1323,7 @@
         <v>0</v>
       </c>
       <c r="F50" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
@@ -1280,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
@@ -1291,7 +1345,7 @@
         <v>0</v>
       </c>
       <c r="F52" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
@@ -1302,7 +1356,7 @@
         <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
@@ -1313,29 +1367,29 @@
         <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>54</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>55</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>0</v>
       </c>
       <c r="F56" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
@@ -1346,7 +1400,10 @@
         <v>0</v>
       </c>
       <c r="F57" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="G57" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
@@ -1357,7 +1414,10 @@
         <v>0</v>
       </c>
       <c r="F58" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="G58" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
@@ -1368,7 +1428,10 @@
         <v>0</v>
       </c>
       <c r="F59" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="G59" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.25">
@@ -1379,63 +1442,84 @@
         <v>0</v>
       </c>
       <c r="F60" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="G60" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
+        <v>65</v>
+      </c>
+      <c r="E61" t="s">
+        <v>0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>66</v>
+      </c>
+      <c r="G61" t="s">
         <v>67</v>
-      </c>
-      <c r="E61" t="s">
-        <v>0</v>
-      </c>
-      <c r="F61" t="s">
-        <v>68</v>
-      </c>
-      <c r="G61" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E62" t="s">
         <v>0</v>
       </c>
       <c r="F62" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G62" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E63" t="s">
         <v>0</v>
       </c>
       <c r="F63" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G63" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E64" t="s">
         <v>0</v>
       </c>
       <c r="F64" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>76</v>
+      </c>
+      <c r="E65" t="s">
+        <v>0</v>
+      </c>
+      <c r="F65" t="s">
+        <v>66</v>
+      </c>
+      <c r="G65" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="G30:G31"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>